<commit_message>
24hr before lab meeting
</commit_message>
<xml_diff>
--- a/neoteny/neoteny.xlsx
+++ b/neoteny/neoteny.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jon/Documents/Salamanders/fossilSalamanders/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jon/Documents/Salamanders/neoteny/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24340" yWindow="1200" windowWidth="28160" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2341,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A351" workbookViewId="0">
-      <selection activeCell="C379" sqref="C379"/>
+    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
+      <selection activeCell="B441" sqref="B441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2372,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <f>0+(0)</f>
+        <f t="shared" ref="C2:C9" si="0">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2384,7 +2384,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <f>0+(0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2396,7 +2396,7 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <f>0+(0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2408,7 +2408,7 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <f>0+(0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2420,7 +2420,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <f>0+(0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2432,7 +2432,7 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <f>0+(0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2444,7 +2444,7 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <f>0+(0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2456,8 +2456,7 @@
         <v>17</v>
       </c>
       <c r="C9">
-        <f>0+(0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2468,7 +2467,7 @@
         <v>19</v>
       </c>
       <c r="C10">
-        <f>2+(0)</f>
+        <f t="shared" ref="C10:C16" si="1">2+(0)</f>
         <v>2</v>
       </c>
     </row>
@@ -2480,7 +2479,7 @@
         <v>20</v>
       </c>
       <c r="C11">
-        <f>2+(0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2492,7 +2491,7 @@
         <v>21</v>
       </c>
       <c r="C12">
-        <f>2+(0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2504,7 +2503,7 @@
         <v>22</v>
       </c>
       <c r="C13">
-        <f>2+(0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2516,7 +2515,7 @@
         <v>24</v>
       </c>
       <c r="C14">
-        <f>2+(0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2528,7 +2527,7 @@
         <v>26</v>
       </c>
       <c r="C15">
-        <f>2+(0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2540,7 +2539,7 @@
         <v>27</v>
       </c>
       <c r="C16">
-        <f>2+(0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2902,7 +2901,7 @@
         <v>81</v>
       </c>
       <c r="C47">
-        <f>2+(0)</f>
+        <f t="shared" ref="C47:C53" si="2">2+(0)</f>
         <v>2</v>
       </c>
     </row>
@@ -2914,7 +2913,7 @@
         <v>82</v>
       </c>
       <c r="C48">
-        <f>2+(0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2926,7 +2925,7 @@
         <v>84</v>
       </c>
       <c r="C49">
-        <f>2+(0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2938,7 +2937,7 @@
         <v>86</v>
       </c>
       <c r="C50">
-        <f>2+(0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2950,7 +2949,7 @@
         <v>88</v>
       </c>
       <c r="C51">
-        <f>2+(0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2962,7 +2961,7 @@
         <v>90</v>
       </c>
       <c r="C52">
-        <f>2+(0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2974,7 +2973,7 @@
         <v>92</v>
       </c>
       <c r="C53">
-        <f>2+(0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3320,7 +3319,7 @@
         <v>141</v>
       </c>
       <c r="C82">
-        <f>0+(0)</f>
+        <f t="shared" ref="C82:C87" si="3">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3332,7 +3331,7 @@
         <v>143</v>
       </c>
       <c r="C83">
-        <f>0+(0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3344,7 +3343,7 @@
         <v>145</v>
       </c>
       <c r="C84">
-        <f>0+(0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3356,7 +3355,7 @@
         <v>147</v>
       </c>
       <c r="C85">
-        <f>0+(0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3368,7 +3367,7 @@
         <v>149</v>
       </c>
       <c r="C86">
-        <f>0+(0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3380,7 +3379,7 @@
         <v>151</v>
       </c>
       <c r="C87">
-        <f>0+(0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3467,7 +3466,7 @@
         <v>161</v>
       </c>
       <c r="C94">
-        <f>0+(0)</f>
+        <f t="shared" ref="C94:C112" si="4">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3479,7 +3478,7 @@
         <v>163</v>
       </c>
       <c r="C95">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3491,7 +3490,7 @@
         <v>165</v>
       </c>
       <c r="C96">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3503,7 +3502,7 @@
         <v>167</v>
       </c>
       <c r="C97">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3515,7 +3514,7 @@
         <v>169</v>
       </c>
       <c r="C98">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3527,7 +3526,7 @@
         <v>171</v>
       </c>
       <c r="C99">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3539,7 +3538,7 @@
         <v>172</v>
       </c>
       <c r="C100">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3551,7 +3550,7 @@
         <v>173</v>
       </c>
       <c r="C101">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3563,7 +3562,7 @@
         <v>175</v>
       </c>
       <c r="C102">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3575,7 +3574,7 @@
         <v>176</v>
       </c>
       <c r="C103">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3587,7 +3586,7 @@
         <v>177</v>
       </c>
       <c r="C104">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3599,7 +3598,7 @@
         <v>178</v>
       </c>
       <c r="C105">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3611,7 +3610,7 @@
         <v>179</v>
       </c>
       <c r="C106">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3623,7 +3622,7 @@
         <v>181</v>
       </c>
       <c r="C107">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3635,7 +3634,7 @@
         <v>182</v>
       </c>
       <c r="C108">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3647,7 +3646,7 @@
         <v>184</v>
       </c>
       <c r="C109">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3659,7 +3658,7 @@
         <v>185</v>
       </c>
       <c r="C110">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3671,7 +3670,7 @@
         <v>186</v>
       </c>
       <c r="C111">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3683,7 +3682,7 @@
         <v>187</v>
       </c>
       <c r="C112">
-        <f>0+(0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3709,7 +3708,7 @@
         <v>190</v>
       </c>
       <c r="C114">
-        <f>0+(0)</f>
+        <f t="shared" ref="C114:C141" si="5">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3721,7 +3720,7 @@
         <v>191</v>
       </c>
       <c r="C115">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3733,7 +3732,7 @@
         <v>192</v>
       </c>
       <c r="C116">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3745,7 +3744,7 @@
         <v>193</v>
       </c>
       <c r="C117">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3757,7 +3756,7 @@
         <v>194</v>
       </c>
       <c r="C118">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3769,7 +3768,7 @@
         <v>195</v>
       </c>
       <c r="C119">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3781,7 +3780,7 @@
         <v>196</v>
       </c>
       <c r="C120">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3793,7 +3792,7 @@
         <v>197</v>
       </c>
       <c r="C121">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3805,7 +3804,7 @@
         <v>198</v>
       </c>
       <c r="C122">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3817,7 +3816,7 @@
         <v>199</v>
       </c>
       <c r="C123">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3829,7 +3828,7 @@
         <v>200</v>
       </c>
       <c r="C124">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3841,7 +3840,7 @@
         <v>201</v>
       </c>
       <c r="C125">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3853,7 +3852,7 @@
         <v>202</v>
       </c>
       <c r="C126">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3865,7 +3864,7 @@
         <v>203</v>
       </c>
       <c r="C127">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3877,7 +3876,7 @@
         <v>204</v>
       </c>
       <c r="C128">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3889,7 +3888,7 @@
         <v>205</v>
       </c>
       <c r="C129">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3901,7 +3900,7 @@
         <v>206</v>
       </c>
       <c r="C130">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3913,7 +3912,7 @@
         <v>207</v>
       </c>
       <c r="C131">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3925,7 +3924,7 @@
         <v>208</v>
       </c>
       <c r="C132">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3937,7 +3936,7 @@
         <v>209</v>
       </c>
       <c r="C133">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3949,7 +3948,7 @@
         <v>210</v>
       </c>
       <c r="C134">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3961,7 +3960,7 @@
         <v>211</v>
       </c>
       <c r="C135">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3973,7 +3972,7 @@
         <v>212</v>
       </c>
       <c r="C136">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3985,7 +3984,7 @@
         <v>213</v>
       </c>
       <c r="C137">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3997,7 +3996,7 @@
         <v>214</v>
       </c>
       <c r="C138">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4009,7 +4008,7 @@
         <v>22</v>
       </c>
       <c r="C139">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4021,7 +4020,7 @@
         <v>215</v>
       </c>
       <c r="C140">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4033,7 +4032,7 @@
         <v>216</v>
       </c>
       <c r="C141">
-        <f>0+(0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4159,7 +4158,7 @@
         <v>226</v>
       </c>
       <c r="C152">
-        <f>0+(0)</f>
+        <f t="shared" ref="C152:C161" si="6">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4171,7 +4170,7 @@
         <v>227</v>
       </c>
       <c r="C153">
-        <f>0+(0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4183,7 +4182,7 @@
         <v>228</v>
       </c>
       <c r="C154">
-        <f>0+(0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4195,7 +4194,7 @@
         <v>229</v>
       </c>
       <c r="C155">
-        <f>0+(0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4207,7 +4206,7 @@
         <v>230</v>
       </c>
       <c r="C156">
-        <f>0+(0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4219,7 +4218,7 @@
         <v>231</v>
       </c>
       <c r="C157">
-        <f>0+(0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4231,7 +4230,7 @@
         <v>232</v>
       </c>
       <c r="C158">
-        <f>0+(0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4243,7 +4242,7 @@
         <v>233</v>
       </c>
       <c r="C159">
-        <f>0+(0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4255,7 +4254,7 @@
         <v>234</v>
       </c>
       <c r="C160">
-        <f>0+(0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4267,7 +4266,7 @@
         <v>235</v>
       </c>
       <c r="C161">
-        <f>0+(0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4342,7 +4341,7 @@
         <v>242</v>
       </c>
       <c r="C167">
-        <f>0+(0)</f>
+        <f t="shared" ref="C167:C183" si="7">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4354,7 +4353,7 @@
         <v>243</v>
       </c>
       <c r="C168">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4366,7 +4365,7 @@
         <v>245</v>
       </c>
       <c r="C169">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4378,7 +4377,7 @@
         <v>246</v>
       </c>
       <c r="C170">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4390,7 +4389,7 @@
         <v>247</v>
       </c>
       <c r="C171">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4402,7 +4401,7 @@
         <v>248</v>
       </c>
       <c r="C172">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4414,7 +4413,7 @@
         <v>249</v>
       </c>
       <c r="C173">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4426,7 +4425,7 @@
         <v>250</v>
       </c>
       <c r="C174">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4438,7 +4437,7 @@
         <v>251</v>
       </c>
       <c r="C175">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4450,7 +4449,7 @@
         <v>252</v>
       </c>
       <c r="C176">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4462,7 +4461,7 @@
         <v>254</v>
       </c>
       <c r="C177">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4474,7 +4473,7 @@
         <v>255</v>
       </c>
       <c r="C178">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4486,7 +4485,7 @@
         <v>256</v>
       </c>
       <c r="C179">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4498,7 +4497,7 @@
         <v>257</v>
       </c>
       <c r="C180">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4510,7 +4509,7 @@
         <v>258</v>
       </c>
       <c r="C181">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4522,7 +4521,7 @@
         <v>259</v>
       </c>
       <c r="C182">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4534,7 +4533,7 @@
         <v>260</v>
       </c>
       <c r="C183">
-        <f>0+(0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4558,7 +4557,7 @@
         <v>214</v>
       </c>
       <c r="C185">
-        <f>0+(0)</f>
+        <f t="shared" ref="C185:C195" si="8">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4570,7 +4569,7 @@
         <v>262</v>
       </c>
       <c r="C186">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4582,7 +4581,7 @@
         <v>264</v>
       </c>
       <c r="C187">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4594,7 +4593,7 @@
         <v>240</v>
       </c>
       <c r="C188">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4606,7 +4605,7 @@
         <v>266</v>
       </c>
       <c r="C189">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4618,7 +4617,7 @@
         <v>267</v>
       </c>
       <c r="C190">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4630,7 +4629,7 @@
         <v>268</v>
       </c>
       <c r="C191">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4642,7 +4641,7 @@
         <v>269</v>
       </c>
       <c r="C192">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4654,7 +4653,7 @@
         <v>270</v>
       </c>
       <c r="C193">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4666,7 +4665,7 @@
         <v>271</v>
       </c>
       <c r="C194">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4678,7 +4677,7 @@
         <v>272</v>
       </c>
       <c r="C195">
-        <f>0+(0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4800,7 +4799,7 @@
         <v>282</v>
       </c>
       <c r="C205">
-        <f>0+(0)</f>
+        <f t="shared" ref="C205:C211" si="9">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4812,7 +4811,7 @@
         <v>283</v>
       </c>
       <c r="C206">
-        <f>0+(0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4824,7 +4823,7 @@
         <v>284</v>
       </c>
       <c r="C207">
-        <f>0+(0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4836,7 +4835,7 @@
         <v>286</v>
       </c>
       <c r="C208">
-        <f>0+(0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4848,7 +4847,7 @@
         <v>288</v>
       </c>
       <c r="C209">
-        <f>0+(0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4860,7 +4859,7 @@
         <v>289</v>
       </c>
       <c r="C210">
-        <f>0+(0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4872,7 +4871,7 @@
         <v>291</v>
       </c>
       <c r="C211">
-        <f>0+(0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4896,7 +4895,7 @@
         <v>293</v>
       </c>
       <c r="C213">
-        <f>0+(0)</f>
+        <f t="shared" ref="C213:C219" si="10">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4908,7 +4907,7 @@
         <v>294</v>
       </c>
       <c r="C214">
-        <f>0+(0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4920,7 +4919,7 @@
         <v>208</v>
       </c>
       <c r="C215">
-        <f>0+(0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4932,7 +4931,7 @@
         <v>295</v>
       </c>
       <c r="C216">
-        <f>0+(0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4944,7 +4943,7 @@
         <v>296</v>
       </c>
       <c r="C217">
-        <f>0+(0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4956,7 +4955,7 @@
         <v>297</v>
       </c>
       <c r="C218">
-        <f>0+(0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4968,7 +4967,7 @@
         <v>298</v>
       </c>
       <c r="C219">
-        <f>0+(0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -5051,7 +5050,7 @@
         <v>306</v>
       </c>
       <c r="C226">
-        <f>0+(0)</f>
+        <f t="shared" ref="C226:C232" si="11">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5063,7 +5062,7 @@
         <v>308</v>
       </c>
       <c r="C227">
-        <f>0+(0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -5075,7 +5074,7 @@
         <v>309</v>
       </c>
       <c r="C228">
-        <f>0+(0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -5087,7 +5086,7 @@
         <v>311</v>
       </c>
       <c r="C229">
-        <f>0+(0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -5099,7 +5098,7 @@
         <v>312</v>
       </c>
       <c r="C230">
-        <f>0+(0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -5111,7 +5110,7 @@
         <v>313</v>
       </c>
       <c r="C231">
-        <f>0+(0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -5123,7 +5122,7 @@
         <v>314</v>
       </c>
       <c r="C232">
-        <f>0+(0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -5242,7 +5241,7 @@
         <v>326</v>
       </c>
       <c r="C242">
-        <f>2+(0)</f>
+        <f t="shared" ref="C242:C247" si="12">2+(0)</f>
         <v>2</v>
       </c>
     </row>
@@ -5254,7 +5253,7 @@
         <v>327</v>
       </c>
       <c r="C243">
-        <f>2+(0)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
     </row>
@@ -5266,7 +5265,7 @@
         <v>328</v>
       </c>
       <c r="C244">
-        <f>2+(0)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
     </row>
@@ -5278,7 +5277,7 @@
         <v>329</v>
       </c>
       <c r="C245">
-        <f>2+(0)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
     </row>
@@ -5290,7 +5289,7 @@
         <v>330</v>
       </c>
       <c r="C246">
-        <f>2+(0)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
     </row>
@@ -5302,7 +5301,7 @@
         <v>331</v>
       </c>
       <c r="C247">
-        <f>2+(0)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
     </row>
@@ -5398,7 +5397,7 @@
         <v>341</v>
       </c>
       <c r="C255">
-        <f>0+(0)</f>
+        <f t="shared" ref="C255:C270" si="13">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5410,7 +5409,7 @@
         <v>343</v>
       </c>
       <c r="C256">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5422,7 +5421,7 @@
         <v>344</v>
       </c>
       <c r="C257">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5434,7 +5433,7 @@
         <v>300</v>
       </c>
       <c r="C258">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5446,7 +5445,7 @@
         <v>345</v>
       </c>
       <c r="C259">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5458,7 +5457,7 @@
         <v>346</v>
       </c>
       <c r="C260">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5470,7 +5469,7 @@
         <v>303</v>
       </c>
       <c r="C261">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5482,7 +5481,7 @@
         <v>347</v>
       </c>
       <c r="C262">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5494,7 +5493,7 @@
         <v>348</v>
       </c>
       <c r="C263">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5506,7 +5505,7 @@
         <v>349</v>
       </c>
       <c r="C264">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5518,7 +5517,7 @@
         <v>350</v>
       </c>
       <c r="C265">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5530,7 +5529,7 @@
         <v>351</v>
       </c>
       <c r="C266">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5542,7 +5541,7 @@
         <v>353</v>
       </c>
       <c r="C267">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5554,7 +5553,7 @@
         <v>355</v>
       </c>
       <c r="C268">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5566,7 +5565,7 @@
         <v>356</v>
       </c>
       <c r="C269">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5578,7 +5577,7 @@
         <v>357</v>
       </c>
       <c r="C270">
-        <f>0+(0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -5604,7 +5603,7 @@
         <v>359</v>
       </c>
       <c r="C272">
-        <f>0+(0)</f>
+        <f t="shared" ref="C272:C303" si="14">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5616,7 +5615,7 @@
         <v>360</v>
       </c>
       <c r="C273">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5628,7 +5627,7 @@
         <v>362</v>
       </c>
       <c r="C274">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5640,7 +5639,7 @@
         <v>364</v>
       </c>
       <c r="C275">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5652,7 +5651,7 @@
         <v>365</v>
       </c>
       <c r="C276">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5664,7 +5663,7 @@
         <v>319</v>
       </c>
       <c r="C277">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5676,7 +5675,7 @@
         <v>366</v>
       </c>
       <c r="C278">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5688,7 +5687,7 @@
         <v>355</v>
       </c>
       <c r="C279">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5700,7 +5699,7 @@
         <v>367</v>
       </c>
       <c r="C280">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5712,7 +5711,7 @@
         <v>368</v>
       </c>
       <c r="C281">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5724,7 +5723,7 @@
         <v>369</v>
       </c>
       <c r="C282">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5736,7 +5735,7 @@
         <v>370</v>
       </c>
       <c r="C283">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5748,7 +5747,7 @@
         <v>371</v>
       </c>
       <c r="C284">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5760,7 +5759,7 @@
         <v>372</v>
       </c>
       <c r="C285">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5772,7 +5771,7 @@
         <v>373</v>
       </c>
       <c r="C286">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5784,7 +5783,7 @@
         <v>374</v>
       </c>
       <c r="C287">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5796,7 +5795,7 @@
         <v>375</v>
       </c>
       <c r="C288">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5808,7 +5807,7 @@
         <v>376</v>
       </c>
       <c r="C289">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5820,7 +5819,7 @@
         <v>377</v>
       </c>
       <c r="C290">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5832,7 +5831,7 @@
         <v>378</v>
       </c>
       <c r="C291">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5844,7 +5843,7 @@
         <v>379</v>
       </c>
       <c r="C292">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5856,7 +5855,7 @@
         <v>380</v>
       </c>
       <c r="C293">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5868,7 +5867,7 @@
         <v>382</v>
       </c>
       <c r="C294">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5880,7 +5879,7 @@
         <v>383</v>
       </c>
       <c r="C295">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5892,7 +5891,7 @@
         <v>384</v>
       </c>
       <c r="C296">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5904,7 +5903,7 @@
         <v>385</v>
       </c>
       <c r="C297">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5916,7 +5915,7 @@
         <v>22</v>
       </c>
       <c r="C298">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5928,7 +5927,7 @@
         <v>386</v>
       </c>
       <c r="C299">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5940,7 +5939,7 @@
         <v>387</v>
       </c>
       <c r="C300">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5952,7 +5951,7 @@
         <v>388</v>
       </c>
       <c r="C301">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5964,7 +5963,7 @@
         <v>389</v>
       </c>
       <c r="C302">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5976,7 +5975,7 @@
         <v>390</v>
       </c>
       <c r="C303">
-        <f>0+(0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -5988,7 +5987,7 @@
         <v>391</v>
       </c>
       <c r="C304">
-        <f>0+(0)</f>
+        <f t="shared" ref="C304:C335" si="15">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6000,7 +5999,7 @@
         <v>392</v>
       </c>
       <c r="C305">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6012,7 +6011,7 @@
         <v>393</v>
       </c>
       <c r="C306">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6024,7 +6023,7 @@
         <v>394</v>
       </c>
       <c r="C307">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6036,7 +6035,7 @@
         <v>395</v>
       </c>
       <c r="C308">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6048,7 +6047,7 @@
         <v>396</v>
       </c>
       <c r="C309">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6060,7 +6059,7 @@
         <v>362</v>
       </c>
       <c r="C310">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6072,7 +6071,7 @@
         <v>397</v>
       </c>
       <c r="C311">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6084,7 +6083,7 @@
         <v>398</v>
       </c>
       <c r="C312">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6096,7 +6095,7 @@
         <v>399</v>
       </c>
       <c r="C313">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6108,7 +6107,7 @@
         <v>400</v>
       </c>
       <c r="C314">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6120,7 +6119,7 @@
         <v>328</v>
       </c>
       <c r="C315">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6132,7 +6131,7 @@
         <v>401</v>
       </c>
       <c r="C316">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6144,7 +6143,7 @@
         <v>402</v>
       </c>
       <c r="C317">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6156,7 +6155,7 @@
         <v>403</v>
       </c>
       <c r="C318">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6168,7 +6167,7 @@
         <v>404</v>
       </c>
       <c r="C319">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6180,7 +6179,7 @@
         <v>405</v>
       </c>
       <c r="C320">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6192,7 +6191,7 @@
         <v>406</v>
       </c>
       <c r="C321">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6204,7 +6203,7 @@
         <v>407</v>
       </c>
       <c r="C322">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6216,7 +6215,7 @@
         <v>408</v>
       </c>
       <c r="C323">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6228,7 +6227,7 @@
         <v>409</v>
       </c>
       <c r="C324">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6240,7 +6239,7 @@
         <v>410</v>
       </c>
       <c r="C325">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6252,7 +6251,7 @@
         <v>411</v>
       </c>
       <c r="C326">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6264,7 +6263,7 @@
         <v>412</v>
       </c>
       <c r="C327">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6276,7 +6275,7 @@
         <v>413</v>
       </c>
       <c r="C328">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6288,7 +6287,7 @@
         <v>414</v>
       </c>
       <c r="C329">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6300,7 +6299,7 @@
         <v>415</v>
       </c>
       <c r="C330">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6312,7 +6311,7 @@
         <v>416</v>
       </c>
       <c r="C331">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6324,7 +6323,7 @@
         <v>417</v>
       </c>
       <c r="C332">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6336,7 +6335,7 @@
         <v>418</v>
       </c>
       <c r="C333">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6348,7 +6347,7 @@
         <v>419</v>
       </c>
       <c r="C334">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6360,7 +6359,7 @@
         <v>420</v>
       </c>
       <c r="C335">
-        <f>0+(0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6372,7 +6371,7 @@
         <v>421</v>
       </c>
       <c r="C336">
-        <f>0+(0)</f>
+        <f t="shared" ref="C336:C352" si="16">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6384,7 +6383,7 @@
         <v>301</v>
       </c>
       <c r="C337">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6396,7 +6395,7 @@
         <v>422</v>
       </c>
       <c r="C338">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6408,7 +6407,7 @@
         <v>423</v>
       </c>
       <c r="C339">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6420,7 +6419,7 @@
         <v>424</v>
       </c>
       <c r="C340">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6432,7 +6431,7 @@
         <v>425</v>
       </c>
       <c r="C341">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6444,7 +6443,7 @@
         <v>426</v>
       </c>
       <c r="C342">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6456,7 +6455,7 @@
         <v>427</v>
       </c>
       <c r="C343">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6468,7 +6467,7 @@
         <v>428</v>
       </c>
       <c r="C344">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6480,7 +6479,7 @@
         <v>429</v>
       </c>
       <c r="C345">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6492,7 +6491,7 @@
         <v>430</v>
       </c>
       <c r="C346">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6504,7 +6503,7 @@
         <v>431</v>
       </c>
       <c r="C347">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6516,7 +6515,7 @@
         <v>433</v>
       </c>
       <c r="C348">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6528,7 +6527,7 @@
         <v>435</v>
       </c>
       <c r="C349">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6540,7 +6539,7 @@
         <v>301</v>
       </c>
       <c r="C350">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6552,7 +6551,7 @@
         <v>437</v>
       </c>
       <c r="C351">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6564,7 +6563,7 @@
         <v>439</v>
       </c>
       <c r="C352">
-        <f>0+(0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6654,7 +6653,7 @@
         <v>448</v>
       </c>
       <c r="C359">
-        <f>0+(0)</f>
+        <f t="shared" ref="C359:C364" si="17">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6666,7 +6665,7 @@
         <v>449</v>
       </c>
       <c r="C360">
-        <f>0+(0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6678,7 +6677,7 @@
         <v>450</v>
       </c>
       <c r="C361">
-        <f>0+(0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6690,7 +6689,7 @@
         <v>451</v>
       </c>
       <c r="C362">
-        <f>0+(0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6702,7 +6701,7 @@
         <v>452</v>
       </c>
       <c r="C363">
-        <f>0+(0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6714,7 +6713,7 @@
         <v>453</v>
       </c>
       <c r="C364">
-        <f>0+(0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6930,7 +6929,7 @@
         <v>364</v>
       </c>
       <c r="C382">
-        <f>0+(0)</f>
+        <f t="shared" ref="C382:C387" si="18">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6942,7 +6941,7 @@
         <v>473</v>
       </c>
       <c r="C383">
-        <f>0+(0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -6954,7 +6953,7 @@
         <v>474</v>
       </c>
       <c r="C384">
-        <f>0+(0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -6966,7 +6965,7 @@
         <v>475</v>
       </c>
       <c r="C385">
-        <f>0+(0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -6978,7 +6977,7 @@
         <v>476</v>
       </c>
       <c r="C386">
-        <f>0+(0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -6990,7 +6989,7 @@
         <v>477</v>
       </c>
       <c r="C387">
-        <f>0+(0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -7016,7 +7015,7 @@
         <v>479</v>
       </c>
       <c r="C389">
-        <f>0+(0)</f>
+        <f t="shared" ref="C389:C420" si="19">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7028,7 +7027,7 @@
         <v>480</v>
       </c>
       <c r="C390">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7040,7 +7039,7 @@
         <v>481</v>
       </c>
       <c r="C391">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7052,7 +7051,7 @@
         <v>482</v>
       </c>
       <c r="C392">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7064,7 +7063,7 @@
         <v>483</v>
       </c>
       <c r="C393">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7076,7 +7075,7 @@
         <v>484</v>
       </c>
       <c r="C394">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7088,7 +7087,7 @@
         <v>485</v>
       </c>
       <c r="C395">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7100,7 +7099,7 @@
         <v>486</v>
       </c>
       <c r="C396">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7112,7 +7111,7 @@
         <v>487</v>
       </c>
       <c r="C397">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7124,7 +7123,7 @@
         <v>488</v>
       </c>
       <c r="C398">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7136,7 +7135,7 @@
         <v>490</v>
       </c>
       <c r="C399">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7148,7 +7147,7 @@
         <v>492</v>
       </c>
       <c r="C400">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7160,7 +7159,7 @@
         <v>493</v>
       </c>
       <c r="C401">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7172,7 +7171,7 @@
         <v>494</v>
       </c>
       <c r="C402">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7184,7 +7183,7 @@
         <v>495</v>
       </c>
       <c r="C403">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7196,7 +7195,7 @@
         <v>496</v>
       </c>
       <c r="C404">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7208,7 +7207,7 @@
         <v>497</v>
       </c>
       <c r="C405">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7220,7 +7219,7 @@
         <v>233</v>
       </c>
       <c r="C406">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7232,7 +7231,7 @@
         <v>499</v>
       </c>
       <c r="C407">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7244,7 +7243,7 @@
         <v>500</v>
       </c>
       <c r="C408">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7256,7 +7255,7 @@
         <v>501</v>
       </c>
       <c r="C409">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7268,7 +7267,7 @@
         <v>502</v>
       </c>
       <c r="C410">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7280,7 +7279,7 @@
         <v>503</v>
       </c>
       <c r="C411">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7292,7 +7291,7 @@
         <v>504</v>
       </c>
       <c r="C412">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7304,7 +7303,7 @@
         <v>505</v>
       </c>
       <c r="C413">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7316,7 +7315,7 @@
         <v>506</v>
       </c>
       <c r="C414">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7328,7 +7327,7 @@
         <v>507</v>
       </c>
       <c r="C415">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7340,7 +7339,7 @@
         <v>508</v>
       </c>
       <c r="C416">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7352,7 +7351,7 @@
         <v>510</v>
       </c>
       <c r="C417">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7364,7 +7363,7 @@
         <v>511</v>
       </c>
       <c r="C418">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7376,7 +7375,7 @@
         <v>512</v>
       </c>
       <c r="C419">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7388,7 +7387,7 @@
         <v>465</v>
       </c>
       <c r="C420">
-        <f>0+(0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7400,7 +7399,7 @@
         <v>514</v>
       </c>
       <c r="C421">
-        <f>0+(0)</f>
+        <f t="shared" ref="C421:C452" si="20">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7412,7 +7411,7 @@
         <v>515</v>
       </c>
       <c r="C422">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7424,7 +7423,7 @@
         <v>516</v>
       </c>
       <c r="C423">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7436,7 +7435,7 @@
         <v>518</v>
       </c>
       <c r="C424">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7448,7 +7447,7 @@
         <v>520</v>
       </c>
       <c r="C425">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7460,7 +7459,7 @@
         <v>521</v>
       </c>
       <c r="C426">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7472,7 +7471,7 @@
         <v>522</v>
       </c>
       <c r="C427">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7484,7 +7483,7 @@
         <v>523</v>
       </c>
       <c r="C428">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7496,7 +7495,7 @@
         <v>524</v>
       </c>
       <c r="C429">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7508,7 +7507,7 @@
         <v>525</v>
       </c>
       <c r="C430">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7520,7 +7519,7 @@
         <v>526</v>
       </c>
       <c r="C431">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7532,7 +7531,7 @@
         <v>527</v>
       </c>
       <c r="C432">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7544,7 +7543,7 @@
         <v>528</v>
       </c>
       <c r="C433">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7556,7 +7555,7 @@
         <v>529</v>
       </c>
       <c r="C434">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7568,7 +7567,7 @@
         <v>530</v>
       </c>
       <c r="C435">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7580,7 +7579,7 @@
         <v>531</v>
       </c>
       <c r="C436">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7592,7 +7591,7 @@
         <v>532</v>
       </c>
       <c r="C437">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7604,7 +7603,7 @@
         <v>533</v>
       </c>
       <c r="C438">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7616,7 +7615,7 @@
         <v>534</v>
       </c>
       <c r="C439">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7628,7 +7627,7 @@
         <v>535</v>
       </c>
       <c r="C440">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7640,7 +7639,7 @@
         <v>536</v>
       </c>
       <c r="C441">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7652,7 +7651,7 @@
         <v>537</v>
       </c>
       <c r="C442">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7664,7 +7663,7 @@
         <v>53</v>
       </c>
       <c r="C443">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7676,7 +7675,7 @@
         <v>538</v>
       </c>
       <c r="C444">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7688,7 +7687,7 @@
         <v>539</v>
       </c>
       <c r="C445">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7700,7 +7699,7 @@
         <v>541</v>
       </c>
       <c r="C446">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7712,7 +7711,7 @@
         <v>542</v>
       </c>
       <c r="C447">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7724,7 +7723,7 @@
         <v>543</v>
       </c>
       <c r="C448">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7736,7 +7735,7 @@
         <v>544</v>
       </c>
       <c r="C449">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7748,7 +7747,7 @@
         <v>545</v>
       </c>
       <c r="C450">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7760,7 +7759,7 @@
         <v>546</v>
       </c>
       <c r="C451">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7772,7 +7771,7 @@
         <v>547</v>
       </c>
       <c r="C452">
-        <f>0+(0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -7784,7 +7783,7 @@
         <v>512</v>
       </c>
       <c r="C453">
-        <f>0+(0)</f>
+        <f t="shared" ref="C453:C484" si="21">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -7796,7 +7795,7 @@
         <v>548</v>
       </c>
       <c r="C454">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7808,7 +7807,7 @@
         <v>549</v>
       </c>
       <c r="C455">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7820,7 +7819,7 @@
         <v>551</v>
       </c>
       <c r="C456">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7832,7 +7831,7 @@
         <v>553</v>
       </c>
       <c r="C457">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7844,7 +7843,7 @@
         <v>554</v>
       </c>
       <c r="C458">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7856,7 +7855,7 @@
         <v>556</v>
       </c>
       <c r="C459">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7868,7 +7867,7 @@
         <v>557</v>
       </c>
       <c r="C460">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7880,7 +7879,7 @@
         <v>558</v>
       </c>
       <c r="C461">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7892,7 +7891,7 @@
         <v>559</v>
       </c>
       <c r="C462">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7904,7 +7903,7 @@
         <v>560</v>
       </c>
       <c r="C463">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7916,7 +7915,7 @@
         <v>561</v>
       </c>
       <c r="C464">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7928,7 +7927,7 @@
         <v>562</v>
       </c>
       <c r="C465">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7940,7 +7939,7 @@
         <v>563</v>
       </c>
       <c r="C466">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7952,7 +7951,7 @@
         <v>565</v>
       </c>
       <c r="C467">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7964,7 +7963,7 @@
         <v>380</v>
       </c>
       <c r="C468">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7976,7 +7975,7 @@
         <v>566</v>
       </c>
       <c r="C469">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7988,7 +7987,7 @@
         <v>567</v>
       </c>
       <c r="C470">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8000,7 +7999,7 @@
         <v>568</v>
       </c>
       <c r="C471">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8012,7 +8011,7 @@
         <v>569</v>
       </c>
       <c r="C472">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8024,7 +8023,7 @@
         <v>570</v>
       </c>
       <c r="C473">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8036,7 +8035,7 @@
         <v>571</v>
       </c>
       <c r="C474">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8048,7 +8047,7 @@
         <v>572</v>
       </c>
       <c r="C475">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8060,7 +8059,7 @@
         <v>573</v>
       </c>
       <c r="C476">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8072,7 +8071,7 @@
         <v>574</v>
       </c>
       <c r="C477">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8084,7 +8083,7 @@
         <v>575</v>
       </c>
       <c r="C478">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8096,7 +8095,7 @@
         <v>576</v>
       </c>
       <c r="C479">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8108,7 +8107,7 @@
         <v>577</v>
       </c>
       <c r="C480">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8120,7 +8119,7 @@
         <v>578</v>
       </c>
       <c r="C481">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8132,7 +8131,7 @@
         <v>579</v>
       </c>
       <c r="C482">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8144,7 +8143,7 @@
         <v>580</v>
       </c>
       <c r="C483">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8156,7 +8155,7 @@
         <v>581</v>
       </c>
       <c r="C484">
-        <f>0+(0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8168,7 +8167,7 @@
         <v>582</v>
       </c>
       <c r="C485">
-        <f>0+(0)</f>
+        <f t="shared" ref="C485:C516" si="22">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8180,7 +8179,7 @@
         <v>583</v>
       </c>
       <c r="C486">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8192,7 +8191,7 @@
         <v>584</v>
       </c>
       <c r="C487">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8204,7 +8203,7 @@
         <v>585</v>
       </c>
       <c r="C488">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8216,7 +8215,7 @@
         <v>586</v>
       </c>
       <c r="C489">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8228,7 +8227,7 @@
         <v>587</v>
       </c>
       <c r="C490">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8240,7 +8239,7 @@
         <v>588</v>
       </c>
       <c r="C491">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8252,7 +8251,7 @@
         <v>589</v>
       </c>
       <c r="C492">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8264,7 +8263,7 @@
         <v>450</v>
       </c>
       <c r="C493">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8276,7 +8275,7 @@
         <v>590</v>
       </c>
       <c r="C494">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8288,7 +8287,7 @@
         <v>592</v>
       </c>
       <c r="C495">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8300,7 +8299,7 @@
         <v>593</v>
       </c>
       <c r="C496">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8312,7 +8311,7 @@
         <v>594</v>
       </c>
       <c r="C497">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8324,7 +8323,7 @@
         <v>595</v>
       </c>
       <c r="C498">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8336,7 +8335,7 @@
         <v>596</v>
       </c>
       <c r="C499">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8348,7 +8347,7 @@
         <v>53</v>
       </c>
       <c r="C500">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8360,7 +8359,7 @@
         <v>597</v>
       </c>
       <c r="C501">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8372,7 +8371,7 @@
         <v>598</v>
       </c>
       <c r="C502">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8384,7 +8383,7 @@
         <v>599</v>
       </c>
       <c r="C503">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8396,7 +8395,7 @@
         <v>600</v>
       </c>
       <c r="C504">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8408,7 +8407,7 @@
         <v>601</v>
       </c>
       <c r="C505">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8420,7 +8419,7 @@
         <v>602</v>
       </c>
       <c r="C506">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8432,7 +8431,7 @@
         <v>603</v>
       </c>
       <c r="C507">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8444,7 +8443,7 @@
         <v>202</v>
       </c>
       <c r="C508">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8456,7 +8455,7 @@
         <v>604</v>
       </c>
       <c r="C509">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8468,7 +8467,7 @@
         <v>605</v>
       </c>
       <c r="C510">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8480,7 +8479,7 @@
         <v>606</v>
       </c>
       <c r="C511">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8492,7 +8491,7 @@
         <v>607</v>
       </c>
       <c r="C512">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8504,7 +8503,7 @@
         <v>608</v>
       </c>
       <c r="C513">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8516,7 +8515,7 @@
         <v>609</v>
       </c>
       <c r="C514">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8528,7 +8527,7 @@
         <v>610</v>
       </c>
       <c r="C515">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8540,7 +8539,7 @@
         <v>611</v>
       </c>
       <c r="C516">
-        <f>0+(0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -8552,7 +8551,7 @@
         <v>612</v>
       </c>
       <c r="C517">
-        <f>0+(0)</f>
+        <f t="shared" ref="C517:C548" si="23">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8564,7 +8563,7 @@
         <v>613</v>
       </c>
       <c r="C518">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8576,7 +8575,7 @@
         <v>614</v>
       </c>
       <c r="C519">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8588,7 +8587,7 @@
         <v>615</v>
       </c>
       <c r="C520">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8600,7 +8599,7 @@
         <v>616</v>
       </c>
       <c r="C521">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8612,7 +8611,7 @@
         <v>617</v>
       </c>
       <c r="C522">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8624,7 +8623,7 @@
         <v>618</v>
       </c>
       <c r="C523">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8636,7 +8635,7 @@
         <v>619</v>
       </c>
       <c r="C524">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8648,7 +8647,7 @@
         <v>500</v>
       </c>
       <c r="C525">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8660,7 +8659,7 @@
         <v>620</v>
       </c>
       <c r="C526">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8672,7 +8671,7 @@
         <v>621</v>
       </c>
       <c r="C527">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8684,7 +8683,7 @@
         <v>622</v>
       </c>
       <c r="C528">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8696,7 +8695,7 @@
         <v>623</v>
       </c>
       <c r="C529">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8708,7 +8707,7 @@
         <v>624</v>
       </c>
       <c r="C530">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8720,7 +8719,7 @@
         <v>625</v>
       </c>
       <c r="C531">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8732,7 +8731,7 @@
         <v>626</v>
       </c>
       <c r="C532">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8744,7 +8743,7 @@
         <v>627</v>
       </c>
       <c r="C533">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8756,7 +8755,7 @@
         <v>628</v>
       </c>
       <c r="C534">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8768,7 +8767,7 @@
         <v>629</v>
       </c>
       <c r="C535">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8780,7 +8779,7 @@
         <v>630</v>
       </c>
       <c r="C536">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8792,7 +8791,7 @@
         <v>631</v>
       </c>
       <c r="C537">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8804,7 +8803,7 @@
         <v>632</v>
       </c>
       <c r="C538">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8816,7 +8815,7 @@
         <v>633</v>
       </c>
       <c r="C539">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8828,7 +8827,7 @@
         <v>634</v>
       </c>
       <c r="C540">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8840,7 +8839,7 @@
         <v>635</v>
       </c>
       <c r="C541">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8852,7 +8851,7 @@
         <v>636</v>
       </c>
       <c r="C542">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8864,7 +8863,7 @@
         <v>637</v>
       </c>
       <c r="C543">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8876,7 +8875,7 @@
         <v>638</v>
       </c>
       <c r="C544">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8888,7 +8887,7 @@
         <v>639</v>
       </c>
       <c r="C545">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8900,7 +8899,7 @@
         <v>640</v>
       </c>
       <c r="C546">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8912,7 +8911,7 @@
         <v>641</v>
       </c>
       <c r="C547">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8924,7 +8923,7 @@
         <v>642</v>
       </c>
       <c r="C548">
-        <f>0+(0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -8936,7 +8935,7 @@
         <v>643</v>
       </c>
       <c r="C549">
-        <f>0+(0)</f>
+        <f t="shared" ref="C549:C559" si="24">0+(0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8948,7 +8947,7 @@
         <v>644</v>
       </c>
       <c r="C550">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -8960,7 +8959,7 @@
         <v>22</v>
       </c>
       <c r="C551">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -8972,7 +8971,7 @@
         <v>645</v>
       </c>
       <c r="C552">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -8984,7 +8983,7 @@
         <v>380</v>
       </c>
       <c r="C553">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -8996,7 +8995,7 @@
         <v>646</v>
       </c>
       <c r="C554">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -9008,7 +9007,7 @@
         <v>647</v>
       </c>
       <c r="C555">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -9020,7 +9019,7 @@
         <v>258</v>
       </c>
       <c r="C556">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -9032,7 +9031,7 @@
         <v>648</v>
       </c>
       <c r="C557">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -9044,7 +9043,7 @@
         <v>649</v>
       </c>
       <c r="C558">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -9056,7 +9055,7 @@
         <v>650</v>
       </c>
       <c r="C559">
-        <f>0+(0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>